<commit_message>
Testing v4 did testing
</commit_message>
<xml_diff>
--- a/v4/documentation/Testing_v4.xlsx
+++ b/v4/documentation/Testing_v4.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matthew.bulley\Team-Infinite\v4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eric.diep\Desktop\Team-Infinite\Team-Infinite\v4\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9200"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="89">
   <si>
     <t>Test group 1</t>
   </si>
@@ -86,18 +86,6 @@
     <t>Requirement M3 states that the exchange IDs must be unique and in format ex:p:q</t>
   </si>
   <si>
-    <t>Output ex:0:0</t>
-  </si>
-  <si>
-    <t>Alert "Exchange ids must be different."</t>
-  </si>
-  <si>
-    <t>Alert "Exchange 2 id is invalid"</t>
-  </si>
-  <si>
-    <t>Alert "Exchange 1 id is invalid"</t>
-  </si>
-  <si>
     <t>Test Size of Grid</t>
   </si>
   <si>
@@ -119,15 +107,9 @@
     <t>Location of Exchanges must be within the grid</t>
   </si>
   <si>
-    <t>Alert "Exchange 1 location is out of range"</t>
-  </si>
-  <si>
     <t>Test Exchange Location 2</t>
   </si>
   <si>
-    <t>Alert "Exchange 2 location is out of range"</t>
-  </si>
-  <si>
     <t>Test for correct ID output</t>
   </si>
   <si>
@@ -188,21 +170,12 @@
     <t>100000 by 100000 grid is displayed</t>
   </si>
   <si>
-    <t>no grid displayed</t>
-  </si>
-  <si>
     <t>ex:0:0 at coordinates [0,0] and ex:0:1 at coordinates [100000,100000]</t>
   </si>
   <si>
-    <t>ex:0:0 and ex:0:1 at coordinates [5,5] with ex:0:1 below</t>
-  </si>
-  <si>
     <t>Exchange 1 ID should be above exchange 2 ID if both have the same position</t>
   </si>
   <si>
-    <t>ex:0:0 and ex:0:1 at coordinates [0,0] with ex:0:1 below ex:0:0 below home</t>
-  </si>
-  <si>
     <t>Test group 3</t>
   </si>
   <si>
@@ -230,9 +203,6 @@
     <t>Exchange AB where [AB] is the exchange number</t>
   </si>
   <si>
-    <t>There should be 99 Exchanges, with one on each position</t>
-  </si>
-  <si>
     <t>User must input at least 2 exchanges</t>
   </si>
   <si>
@@ -260,7 +230,67 @@
     <t>Exchange 2 capacity</t>
   </si>
   <si>
-    <t>Alert</t>
+    <t>Output message "Nearest exchange: ex:0:1, distance: 10"</t>
+  </si>
+  <si>
+    <t>Alert "Cannot add exchange because its id is not unique."</t>
+  </si>
+  <si>
+    <t>Cannot insert value higher than 10 for exchange id index</t>
+  </si>
+  <si>
+    <t>Location [0,0] is out of the grid range [0,0].</t>
+  </si>
+  <si>
+    <t>Output message "Nearest exchange: ex:0:1, distance: 20"</t>
+  </si>
+  <si>
+    <t>Output message "Nearest exchange: ex:0:0, distance: 20"</t>
+  </si>
+  <si>
+    <t>Alert "Location [20,19] is out of the grid range [20,20]."</t>
+  </si>
+  <si>
+    <t>Alert "Location [19,20] is out of the grid range [20,20]."</t>
+  </si>
+  <si>
+    <t>Alert "Location [20,20] is out of the grid range [20,20]."</t>
+  </si>
+  <si>
+    <t>Output message "Nearest exchange: ex:0:0, distance: 0"</t>
+  </si>
+  <si>
+    <t>Alert "Location [-1,0] is out of the grid range [20,20]."</t>
+  </si>
+  <si>
+    <t>Alert "Location [0,-1] is out of the grid range [20,20]."</t>
+  </si>
+  <si>
+    <t>Alert "Location [-1,-1] is out of the grid range [20,20]."</t>
+  </si>
+  <si>
+    <t>Output message "Nearest exchange: ex:0:1, distance: 0"</t>
+  </si>
+  <si>
+    <t>Exchange 1  capacity</t>
+  </si>
+  <si>
+    <t>Alert "Location [0,0] is out of the grid range [0,0]."</t>
+  </si>
+  <si>
+    <t>ex:0:0 at coordinates [5,5]</t>
+  </si>
+  <si>
+    <t>Alert "Cannot add more than 99 exchanges."</t>
+  </si>
+  <si>
+    <t>Allows Input</t>
+  </si>
+  <si>
+    <t>Message " Nearest exchange: ex:0:1, distance: 10"</t>
+  </si>
+  <si>
+    <t>Alert "Capacity must be between 0 and 999."</t>
   </si>
 </sst>
 </file>
@@ -317,7 +347,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="46">
+  <borders count="49">
     <border>
       <left/>
       <right/>
@@ -892,6 +922,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -899,7 +960,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1002,11 +1063,8 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1032,6 +1090,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="42" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1041,14 +1105,17 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="44" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="46" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="47" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="48" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1434,70 +1501,72 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R77"/>
+  <dimension ref="A1:S78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="30" zoomScaleNormal="30" workbookViewId="0">
-      <selection activeCell="S1" sqref="A1:S76"/>
+    <sheetView tabSelected="1" zoomScale="71" zoomScaleNormal="30" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="84.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="84.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.81640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="25.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.81640625" customWidth="1"/>
-    <col min="15" max="15" width="18.7265625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.85546875" customWidth="1"/>
+    <col min="15" max="15" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A3" s="68" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="70" t="s">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="67" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="72" t="s">
+      <c r="C3" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="77" t="s">
+      <c r="D3" s="79" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="78"/>
-      <c r="F3" s="78"/>
-      <c r="G3" s="78"/>
-      <c r="H3" s="78"/>
-      <c r="I3" s="78"/>
-      <c r="J3" s="78"/>
-      <c r="K3" s="78"/>
-      <c r="L3" s="78"/>
-      <c r="M3" s="79"/>
-      <c r="N3" s="64" t="s">
-        <v>5</v>
-      </c>
-      <c r="O3" s="64" t="s">
+      <c r="E3" s="80"/>
+      <c r="F3" s="80"/>
+      <c r="G3" s="80"/>
+      <c r="H3" s="80"/>
+      <c r="I3" s="80"/>
+      <c r="J3" s="80"/>
+      <c r="K3" s="80"/>
+      <c r="L3" s="80"/>
+      <c r="M3" s="80"/>
+      <c r="N3" s="80"/>
+      <c r="O3" s="81"/>
+      <c r="P3" s="73" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q3" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="P3" s="66" t="s">
+      <c r="R3" s="65" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A4" s="69"/>
-      <c r="B4" s="71"/>
-      <c r="C4" s="73"/>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="68"/>
+      <c r="B4" s="70"/>
+      <c r="C4" s="72"/>
       <c r="D4" s="4" t="s">
         <v>8</v>
       </c>
@@ -1517,22 +1586,28 @@
         <v>13</v>
       </c>
       <c r="J4" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="K4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="L4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="L4" s="5" t="s">
+      <c r="M4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="M4" s="6" t="s">
+      <c r="N4" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="N4" s="65"/>
-      <c r="O4" s="65"/>
-      <c r="P4" s="67"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="O4" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="P4" s="74"/>
+      <c r="Q4" s="74"/>
+      <c r="R4" s="66"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>1.1000000000000001</v>
       </c>
@@ -1564,24 +1639,32 @@
         <v>0</v>
       </c>
       <c r="K5" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L5" s="10">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M5" s="10">
         <v>5</v>
       </c>
-      <c r="N5" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="O5" s="12"/>
-      <c r="P5" s="13" t="str">
-        <f>IF(O5=N5,"PASS","FAIL")</f>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="N5" s="10">
+        <v>5</v>
+      </c>
+      <c r="O5" s="18">
+        <v>0</v>
+      </c>
+      <c r="P5" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q5" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="R5" s="13" t="str">
+        <f>IF(Q5=P5,"PASS","FAIL")</f>
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="14"/>
       <c r="B6" s="15"/>
       <c r="C6" s="16"/>
@@ -1610,21 +1693,29 @@
         <v>0</v>
       </c>
       <c r="L6" s="18">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="M6" s="18">
         <v>5</v>
       </c>
-      <c r="N6" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="O6" s="12"/>
-      <c r="P6" s="13" t="str">
-        <f t="shared" ref="P6:P33" si="0">IF(O6=N6,"PASS","FAIL")</f>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="N6" s="18">
+        <v>5</v>
+      </c>
+      <c r="O6" s="18">
+        <v>0</v>
+      </c>
+      <c r="P6" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q6" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="R6" s="13" t="str">
+        <f t="shared" ref="R6:R33" si="0">IF(Q6=P6,"PASS","FAIL")</f>
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
       <c r="B7" s="15"/>
       <c r="C7" s="16"/>
@@ -1647,27 +1738,35 @@
         <v>15</v>
       </c>
       <c r="J7" s="18">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="K7" s="18">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L7" s="18">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="M7" s="18">
         <v>5</v>
       </c>
-      <c r="N7" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="O7" s="12"/>
-      <c r="P7" s="13" t="str">
+      <c r="N7" s="18">
+        <v>5</v>
+      </c>
+      <c r="O7" s="18">
+        <v>0</v>
+      </c>
+      <c r="P7" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q7" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="R7" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="19"/>
       <c r="B8" s="20"/>
       <c r="C8" s="21"/>
@@ -1696,70 +1795,84 @@
         <v>0</v>
       </c>
       <c r="L8" s="23">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="M8" s="23">
         <v>5</v>
       </c>
-      <c r="N8" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="O8" s="24"/>
-      <c r="P8" s="13" t="str">
+      <c r="N8" s="23">
+        <v>5</v>
+      </c>
+      <c r="O8" s="18">
+        <v>0</v>
+      </c>
+      <c r="P8" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q8" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="R8" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="14">
+        <v>1.2</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="25">
+        <v>100000</v>
+      </c>
+      <c r="E9" s="26">
+        <v>100000</v>
+      </c>
+      <c r="F9" s="26">
+        <v>0</v>
+      </c>
+      <c r="G9" s="26">
+        <v>0</v>
+      </c>
+      <c r="H9" s="26">
+        <v>10</v>
+      </c>
+      <c r="I9" s="26">
+        <v>15</v>
+      </c>
+      <c r="J9" s="26">
+        <v>0</v>
+      </c>
+      <c r="K9" s="26">
+        <v>0</v>
+      </c>
+      <c r="L9" s="26">
+        <v>1</v>
+      </c>
+      <c r="M9" s="26">
+        <v>5</v>
+      </c>
+      <c r="N9" s="26">
+        <v>5</v>
+      </c>
+      <c r="O9" s="18">
+        <v>0</v>
+      </c>
+      <c r="P9" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q9" s="27"/>
+      <c r="R9" s="13" t="str">
         <f t="shared" si="0"/>
         <v>FAIL</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="14">
-        <v>1.2</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="25">
-        <v>100000</v>
-      </c>
-      <c r="E9" s="26">
-        <v>100000</v>
-      </c>
-      <c r="F9" s="26">
-        <v>0</v>
-      </c>
-      <c r="G9" s="26">
-        <v>0</v>
-      </c>
-      <c r="H9" s="26">
-        <v>10</v>
-      </c>
-      <c r="I9" s="26">
-        <v>15</v>
-      </c>
-      <c r="J9" s="26">
-        <v>0</v>
-      </c>
-      <c r="K9" s="26">
-        <v>1</v>
-      </c>
-      <c r="L9" s="26">
-        <v>5</v>
-      </c>
-      <c r="M9" s="26">
-        <v>5</v>
-      </c>
-      <c r="N9" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="O9" s="27"/>
-      <c r="P9" s="13" t="str">
-        <f t="shared" si="0"/>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="14"/>
       <c r="B10" s="16"/>
       <c r="C10" s="16"/>
@@ -1785,24 +1898,30 @@
         <v>0</v>
       </c>
       <c r="K10" s="29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L10" s="29">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M10" s="29">
         <v>5</v>
       </c>
-      <c r="N10" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="O10" s="30"/>
-      <c r="P10" s="13" t="str">
+      <c r="N10" s="29">
+        <v>5</v>
+      </c>
+      <c r="O10" s="18">
+        <v>0</v>
+      </c>
+      <c r="P10" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q10" s="30"/>
+      <c r="R10" s="13" t="str">
         <f t="shared" si="0"/>
         <v>FAIL</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="14"/>
       <c r="B11" s="16"/>
       <c r="C11" s="16"/>
@@ -1828,24 +1947,30 @@
         <v>0</v>
       </c>
       <c r="K11" s="29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L11" s="29">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M11" s="29">
         <v>5</v>
       </c>
-      <c r="N11" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="O11" s="30"/>
-      <c r="P11" s="13" t="str">
+      <c r="N11" s="29">
+        <v>5</v>
+      </c>
+      <c r="O11" s="18">
+        <v>0</v>
+      </c>
+      <c r="P11" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q11" s="30"/>
+      <c r="R11" s="13" t="str">
         <f t="shared" si="0"/>
         <v>FAIL</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="14"/>
       <c r="B12" s="16"/>
       <c r="C12" s="16"/>
@@ -1871,24 +1996,30 @@
         <v>0</v>
       </c>
       <c r="K12" s="29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L12" s="29">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M12" s="29">
         <v>5</v>
       </c>
-      <c r="N12" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="O12" s="30"/>
-      <c r="P12" s="13" t="str">
+      <c r="N12" s="29">
+        <v>5</v>
+      </c>
+      <c r="O12" s="18">
+        <v>0</v>
+      </c>
+      <c r="P12" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q12" s="30"/>
+      <c r="R12" s="13" t="str">
         <f t="shared" si="0"/>
         <v>FAIL</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
       <c r="B13" s="16"/>
       <c r="C13" s="16"/>
@@ -1920,18 +2051,26 @@
         <v>0</v>
       </c>
       <c r="M13" s="29">
-        <v>5</v>
-      </c>
-      <c r="N13" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="O13" s="30"/>
-      <c r="P13" s="13" t="str">
+        <v>0</v>
+      </c>
+      <c r="N13" s="29">
+        <v>0</v>
+      </c>
+      <c r="O13" s="18">
+        <v>0</v>
+      </c>
+      <c r="P13" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q13" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="R13" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="14"/>
       <c r="B14" s="16"/>
       <c r="C14" s="16"/>
@@ -1948,33 +2087,41 @@
         <v>0</v>
       </c>
       <c r="H14" s="29">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="I14" s="29">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="J14" s="29">
         <v>0</v>
       </c>
       <c r="K14" s="29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L14" s="29">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M14" s="29">
-        <v>5</v>
-      </c>
-      <c r="N14" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="O14" s="30"/>
-      <c r="P14" s="13" t="str">
+        <v>0</v>
+      </c>
+      <c r="N14" s="29">
+        <v>0</v>
+      </c>
+      <c r="O14" s="18">
+        <v>0</v>
+      </c>
+      <c r="P14" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q14" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="R14" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="19"/>
       <c r="B15" s="21"/>
       <c r="C15" s="21"/>
@@ -1991,41 +2138,49 @@
         <v>0</v>
       </c>
       <c r="H15" s="32">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="I15" s="32">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="J15" s="32">
         <v>0</v>
       </c>
       <c r="K15" s="32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L15" s="32">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M15" s="32">
-        <v>5</v>
-      </c>
-      <c r="N15" s="33" t="s">
-        <v>28</v>
-      </c>
-      <c r="O15" s="33"/>
-      <c r="P15" s="13" t="str">
+        <v>0</v>
+      </c>
+      <c r="N15" s="32">
+        <v>0</v>
+      </c>
+      <c r="O15" s="18">
+        <v>0</v>
+      </c>
+      <c r="P15" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q15" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="R15" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <v>1.3</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D16" s="25">
         <v>20</v>
@@ -2040,33 +2195,41 @@
         <v>0</v>
       </c>
       <c r="H16" s="26">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I16" s="26">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J16" s="26">
         <v>0</v>
       </c>
       <c r="K16" s="26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L16" s="26">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="M16" s="26">
         <v>10</v>
       </c>
-      <c r="N16" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="O16" s="27"/>
-      <c r="P16" s="13" t="str">
+      <c r="N16" s="26">
+        <v>10</v>
+      </c>
+      <c r="O16" s="18">
+        <v>0</v>
+      </c>
+      <c r="P16" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q16" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="R16" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="14"/>
       <c r="B17" s="16"/>
       <c r="C17" s="16"/>
@@ -2083,33 +2246,41 @@
         <v>0</v>
       </c>
       <c r="H17" s="29">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I17" s="29">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J17" s="29">
         <v>0</v>
       </c>
       <c r="K17" s="29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L17" s="29">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="M17" s="29">
         <v>10</v>
       </c>
-      <c r="N17" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="O17" s="30"/>
-      <c r="P17" s="13" t="str">
+      <c r="N17" s="29">
+        <v>10</v>
+      </c>
+      <c r="O17" s="18">
+        <v>0</v>
+      </c>
+      <c r="P17" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q17" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="R17" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="14"/>
       <c r="B18" s="16"/>
       <c r="C18" s="16"/>
@@ -2126,33 +2297,41 @@
         <v>0</v>
       </c>
       <c r="H18" s="29">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I18" s="29">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J18" s="29">
         <v>0</v>
       </c>
       <c r="K18" s="29">
-        <v>1</v>
-      </c>
-      <c r="L18" s="26">
-        <v>10</v>
+        <v>0</v>
+      </c>
+      <c r="L18" s="29">
+        <v>1</v>
       </c>
       <c r="M18" s="26">
         <v>10</v>
       </c>
-      <c r="N18" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="O18" s="30"/>
-      <c r="P18" s="13" t="str">
+      <c r="N18" s="26">
+        <v>10</v>
+      </c>
+      <c r="O18" s="18">
+        <v>0</v>
+      </c>
+      <c r="P18" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q18" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="R18" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
       <c r="B19" s="16"/>
       <c r="C19" s="16"/>
@@ -2169,33 +2348,41 @@
         <v>0</v>
       </c>
       <c r="H19" s="29">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I19" s="29">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J19" s="29">
         <v>0</v>
       </c>
       <c r="K19" s="29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L19" s="29">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="M19" s="29">
         <v>10</v>
       </c>
-      <c r="N19" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="O19" s="30"/>
-      <c r="P19" s="13" t="str">
+      <c r="N19" s="29">
+        <v>10</v>
+      </c>
+      <c r="O19" s="18">
+        <v>0</v>
+      </c>
+      <c r="P19" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q19" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="R19" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="14"/>
       <c r="B20" s="16"/>
       <c r="C20" s="16"/>
@@ -2221,24 +2408,32 @@
         <v>0</v>
       </c>
       <c r="K20" s="29">
-        <v>1</v>
-      </c>
-      <c r="L20" s="26">
-        <v>10</v>
+        <v>0</v>
+      </c>
+      <c r="L20" s="29">
+        <v>1</v>
       </c>
       <c r="M20" s="26">
         <v>10</v>
       </c>
-      <c r="N20" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="O20" s="30"/>
-      <c r="P20" s="13" t="str">
+      <c r="N20" s="26">
+        <v>10</v>
+      </c>
+      <c r="O20" s="18">
+        <v>0</v>
+      </c>
+      <c r="P20" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q20" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="R20" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="14"/>
       <c r="B21" s="16"/>
       <c r="C21" s="16"/>
@@ -2264,24 +2459,32 @@
         <v>0</v>
       </c>
       <c r="K21" s="29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L21" s="29">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="M21" s="29">
         <v>10</v>
       </c>
-      <c r="N21" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="O21" s="30"/>
-      <c r="P21" s="13" t="str">
+      <c r="N21" s="29">
+        <v>10</v>
+      </c>
+      <c r="O21" s="18">
+        <v>0</v>
+      </c>
+      <c r="P21" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q21" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="R21" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="14"/>
       <c r="B22" s="16"/>
       <c r="C22" s="16"/>
@@ -2307,24 +2510,32 @@
         <v>0</v>
       </c>
       <c r="K22" s="29">
-        <v>1</v>
-      </c>
-      <c r="L22" s="26">
-        <v>10</v>
+        <v>0</v>
+      </c>
+      <c r="L22" s="29">
+        <v>1</v>
       </c>
       <c r="M22" s="26">
         <v>10</v>
       </c>
-      <c r="N22" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="O22" s="30"/>
-      <c r="P22" s="13" t="str">
+      <c r="N22" s="26">
+        <v>10</v>
+      </c>
+      <c r="O22" s="18">
+        <v>0</v>
+      </c>
+      <c r="P22" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q22" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="R22" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="14"/>
       <c r="B23" s="16"/>
       <c r="C23" s="16"/>
@@ -2350,27 +2561,35 @@
         <v>0</v>
       </c>
       <c r="K23" s="29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L23" s="29">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="M23" s="29">
         <v>10</v>
       </c>
-      <c r="N23" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="O23" s="30"/>
-      <c r="P23" s="13" t="str">
+      <c r="N23" s="29">
+        <v>10</v>
+      </c>
+      <c r="O23" s="18">
+        <v>0</v>
+      </c>
+      <c r="P23" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q23" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="R23" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="14"/>
       <c r="B24" s="16" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C24" s="16"/>
       <c r="D24" s="28">
@@ -2395,24 +2614,32 @@
         <v>0</v>
       </c>
       <c r="K24" s="29">
-        <v>1</v>
-      </c>
-      <c r="L24" s="26">
-        <v>20</v>
+        <v>0</v>
+      </c>
+      <c r="L24" s="29">
+        <v>1</v>
       </c>
       <c r="M24" s="26">
-        <v>20</v>
-      </c>
-      <c r="N24" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="O24" s="30"/>
-      <c r="P24" s="13" t="str">
+        <v>19</v>
+      </c>
+      <c r="N24" s="26">
+        <v>19</v>
+      </c>
+      <c r="O24" s="18">
+        <v>0</v>
+      </c>
+      <c r="P24" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q24" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="R24" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="14"/>
       <c r="B25" s="16"/>
       <c r="C25" s="16"/>
@@ -2438,24 +2665,32 @@
         <v>0</v>
       </c>
       <c r="K25" s="29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L25" s="29">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="M25" s="29">
         <v>20</v>
       </c>
-      <c r="N25" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="O25" s="30"/>
-      <c r="P25" s="13" t="str">
+      <c r="N25" s="29">
+        <v>19</v>
+      </c>
+      <c r="O25" s="18">
+        <v>0</v>
+      </c>
+      <c r="P25" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q25" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="R25" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="14"/>
       <c r="B26" s="16"/>
       <c r="C26" s="16"/>
@@ -2481,24 +2716,32 @@
         <v>0</v>
       </c>
       <c r="K26" s="29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L26" s="29">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="M26" s="29">
-        <v>21</v>
-      </c>
-      <c r="N26" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="O26" s="30"/>
-      <c r="P26" s="13" t="str">
+        <v>19</v>
+      </c>
+      <c r="N26" s="29">
+        <v>20</v>
+      </c>
+      <c r="O26" s="18">
+        <v>0</v>
+      </c>
+      <c r="P26" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q26" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="R26" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="14"/>
       <c r="B27" s="16"/>
       <c r="C27" s="16"/>
@@ -2524,24 +2767,32 @@
         <v>0</v>
       </c>
       <c r="K27" s="29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L27" s="29">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="M27" s="29">
-        <v>21</v>
-      </c>
-      <c r="N27" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="O27" s="30"/>
-      <c r="P27" s="13" t="str">
+        <v>20</v>
+      </c>
+      <c r="N27" s="29">
+        <v>20</v>
+      </c>
+      <c r="O27" s="18">
+        <v>0</v>
+      </c>
+      <c r="P27" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q27" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="R27" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="14"/>
       <c r="B28" s="16"/>
       <c r="C28" s="16"/>
@@ -2567,24 +2818,32 @@
         <v>0</v>
       </c>
       <c r="K28" s="29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L28" s="29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M28" s="29">
         <v>0</v>
       </c>
-      <c r="N28" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="O28" s="30"/>
-      <c r="P28" s="13" t="str">
+      <c r="N28" s="29">
+        <v>0</v>
+      </c>
+      <c r="O28" s="18">
+        <v>0</v>
+      </c>
+      <c r="P28" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q28" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="R28" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="14"/>
       <c r="B29" s="16"/>
       <c r="C29" s="16"/>
@@ -2610,24 +2869,32 @@
         <v>0</v>
       </c>
       <c r="K29" s="29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L29" s="29">
+        <v>1</v>
+      </c>
+      <c r="M29" s="29">
         <v>-1</v>
       </c>
-      <c r="M29" s="29">
-        <v>0</v>
-      </c>
-      <c r="N29" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="O29" s="30"/>
-      <c r="P29" s="13" t="str">
+      <c r="N29" s="29">
+        <v>0</v>
+      </c>
+      <c r="O29" s="18">
+        <v>0</v>
+      </c>
+      <c r="P29" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q29" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="R29" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="14"/>
       <c r="B30" s="16"/>
       <c r="C30" s="16"/>
@@ -2653,24 +2920,32 @@
         <v>0</v>
       </c>
       <c r="K30" s="29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L30" s="29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M30" s="29">
+        <v>0</v>
+      </c>
+      <c r="N30" s="29">
         <v>-1</v>
       </c>
-      <c r="N30" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="O30" s="30"/>
-      <c r="P30" s="13" t="str">
+      <c r="O30" s="18">
+        <v>0</v>
+      </c>
+      <c r="P30" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q30" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="R30" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="19"/>
       <c r="B31" s="21"/>
       <c r="C31" s="21"/>
@@ -2696,32 +2971,40 @@
         <v>0</v>
       </c>
       <c r="K31" s="32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L31" s="32">
+        <v>1</v>
+      </c>
+      <c r="M31" s="32">
         <v>-1</v>
       </c>
-      <c r="M31" s="34">
+      <c r="N31" s="34">
         <v>-1</v>
       </c>
-      <c r="N31" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="O31" s="30"/>
-      <c r="P31" s="13" t="str">
+      <c r="O31" s="18">
+        <v>0</v>
+      </c>
+      <c r="P31" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q31" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="R31" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A32" s="14">
         <v>1.4</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D32" s="18">
         <v>20</v>
@@ -2745,28 +3028,36 @@
         <v>0</v>
       </c>
       <c r="K32" s="26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L32" s="26">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M32" s="26">
         <v>5</v>
       </c>
-      <c r="N32" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="O32" s="12"/>
-      <c r="P32" s="13" t="str">
+      <c r="N32" s="26">
+        <v>5</v>
+      </c>
+      <c r="O32" s="18">
+        <v>0</v>
+      </c>
+      <c r="P32" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q32" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="R32" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" s="14"/>
       <c r="B33" s="16"/>
       <c r="C33" s="16" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D33" s="18">
         <v>20</v>
@@ -2790,36 +3081,44 @@
         <v>0</v>
       </c>
       <c r="K33" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L33" s="18">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="M33" s="18">
         <v>10</v>
       </c>
-      <c r="N33" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="O33" s="12"/>
-      <c r="P33" s="13" t="str">
+      <c r="N33" s="18">
+        <v>10</v>
+      </c>
+      <c r="O33" s="18">
+        <v>0</v>
+      </c>
+      <c r="P33" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q33" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="R33" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A37" s="68" t="s">
-        <v>1</v>
-      </c>
-      <c r="B37" s="70" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A37" s="67" t="s">
+        <v>1</v>
+      </c>
+      <c r="B37" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="C37" s="72" t="s">
+      <c r="C37" s="71" t="s">
         <v>3</v>
       </c>
       <c r="D37" s="35" t="s">
@@ -2830,24 +3129,26 @@
       <c r="G37" s="36"/>
       <c r="H37" s="36"/>
       <c r="I37" s="36"/>
-      <c r="J37" s="36"/>
+      <c r="J37" s="64"/>
       <c r="K37" s="36"/>
       <c r="L37" s="36"/>
-      <c r="M37" s="37"/>
-      <c r="N37" s="64" t="s">
-        <v>5</v>
-      </c>
-      <c r="O37" s="64" t="s">
+      <c r="M37" s="36"/>
+      <c r="N37" s="37"/>
+      <c r="O37" s="78"/>
+      <c r="P37" s="73" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q37" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="P37" s="66" t="s">
+      <c r="R37" s="65" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A38" s="69"/>
-      <c r="B38" s="71"/>
-      <c r="C38" s="73"/>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A38" s="68"/>
+      <c r="B38" s="70"/>
+      <c r="C38" s="72"/>
       <c r="D38" s="4" t="s">
         <v>8</v>
       </c>
@@ -2867,30 +3168,36 @@
         <v>13</v>
       </c>
       <c r="J38" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="K38" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="K38" s="5" t="s">
+      <c r="L38" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="L38" s="5" t="s">
+      <c r="M38" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="M38" s="6" t="s">
+      <c r="N38" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="N38" s="65"/>
-      <c r="O38" s="65"/>
-      <c r="P38" s="67"/>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="O38" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="P38" s="74"/>
+      <c r="Q38" s="74"/>
+      <c r="R38" s="66"/>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" s="14">
         <v>2.1</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C39" s="16" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D39" s="18">
         <v>20</v>
@@ -2914,24 +3221,32 @@
         <v>0</v>
       </c>
       <c r="K39" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L39" s="18">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M39" s="18">
         <v>5</v>
       </c>
-      <c r="N39" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="O39" s="11"/>
-      <c r="P39" s="13" t="str">
-        <f>IF(O39=N39,"PASS","FAIL")</f>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="N39" s="18">
+        <v>5</v>
+      </c>
+      <c r="O39" s="18">
+        <v>0</v>
+      </c>
+      <c r="P39" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q39" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="R39" s="13" t="str">
+        <f>IF(Q39=P39,"PASS","FAIL")</f>
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="2"/>
       <c r="C40" s="3"/>
@@ -2957,24 +3272,30 @@
         <v>0</v>
       </c>
       <c r="K40" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L40" s="18">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M40" s="18">
         <v>5</v>
       </c>
-      <c r="N40" s="41" t="s">
-        <v>53</v>
-      </c>
-      <c r="O40" s="41"/>
-      <c r="P40" s="13" t="str">
-        <f t="shared" ref="P40:P41" si="1">IF(O40=N40,"PASS","FAIL")</f>
+      <c r="N40" s="18">
+        <v>5</v>
+      </c>
+      <c r="O40" s="18">
+        <v>0</v>
+      </c>
+      <c r="P40" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q40" s="41"/>
+      <c r="R40" s="13" t="str">
+        <f t="shared" ref="R40:R41" si="1">IF(Q40=P40,"PASS","FAIL")</f>
         <v>FAIL</v>
       </c>
     </row>
-    <row r="41" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="42"/>
       <c r="B41" s="43"/>
       <c r="C41" s="44"/>
@@ -3000,33 +3321,41 @@
         <v>0</v>
       </c>
       <c r="K41" s="32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L41" s="32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M41" s="32">
         <v>0</v>
       </c>
-      <c r="N41" s="45" t="s">
-        <v>54</v>
-      </c>
-      <c r="O41" s="45"/>
-      <c r="P41" s="51" t="str">
+      <c r="N41" s="32">
+        <v>0</v>
+      </c>
+      <c r="O41" s="18">
+        <v>0</v>
+      </c>
+      <c r="P41" s="45" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q41" s="45" t="s">
+        <v>83</v>
+      </c>
+      <c r="R41" s="51" t="str">
         <f t="shared" si="1"/>
-        <v>FAIL</v>
-      </c>
-      <c r="Q41" s="39"/>
-    </row>
-    <row r="42" spans="1:17" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+        <v>PASS</v>
+      </c>
+      <c r="S41" s="39"/>
+    </row>
+    <row r="42" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A42" s="48">
         <v>2.2000000000000002</v>
       </c>
       <c r="B42" s="47" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C42" s="49" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D42" s="18">
         <v>20</v>
@@ -3050,24 +3379,32 @@
         <v>0</v>
       </c>
       <c r="K42" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L42" s="18">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M42" s="18">
         <v>5</v>
       </c>
-      <c r="N42" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="O42" s="12"/>
-      <c r="P42" s="53" t="str">
-        <f>IF(O42=N42,"PASS","FAIL")</f>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="N42" s="18">
+        <v>5</v>
+      </c>
+      <c r="O42" s="18">
+        <v>0</v>
+      </c>
+      <c r="P42" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q42" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="R42" s="53" t="str">
+        <f>IF(Q42=P42,"PASS","FAIL")</f>
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="2"/>
       <c r="C43" s="3"/>
@@ -3093,28 +3430,34 @@
         <v>0</v>
       </c>
       <c r="K43" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L43" s="18">
-        <v>100000</v>
+        <v>1</v>
       </c>
       <c r="M43" s="18">
         <v>100000</v>
       </c>
-      <c r="N43" s="40" t="s">
-        <v>55</v>
-      </c>
-      <c r="O43" s="40"/>
-      <c r="P43" s="38" t="str">
-        <f t="shared" ref="P43:P44" si="2">IF(O43=N43,"PASS","FAIL")</f>
+      <c r="N43" s="18">
+        <v>100000</v>
+      </c>
+      <c r="O43" s="18">
+        <v>0</v>
+      </c>
+      <c r="P43" s="40" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q43" s="40"/>
+      <c r="R43" s="38" t="str">
+        <f t="shared" ref="R43:R44" si="2">IF(Q43=P43,"PASS","FAIL")</f>
         <v>FAIL</v>
       </c>
     </row>
-    <row r="44" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="42"/>
       <c r="B44" s="43"/>
       <c r="C44" s="44" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="D44" s="32">
         <v>20</v>
@@ -3138,32 +3481,40 @@
         <v>0</v>
       </c>
       <c r="K44" s="32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L44" s="32">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M44" s="32">
         <v>5</v>
       </c>
-      <c r="N44" s="45" t="s">
-        <v>56</v>
-      </c>
-      <c r="O44" s="45"/>
-      <c r="P44" s="51" t="str">
+      <c r="N44" s="32">
+        <v>5</v>
+      </c>
+      <c r="O44" s="18">
+        <v>0</v>
+      </c>
+      <c r="P44" s="45" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q44" s="45" t="s">
+        <v>84</v>
+      </c>
+      <c r="R44" s="51" t="str">
         <f t="shared" si="2"/>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="45" spans="1:17" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="19">
         <v>2.2999999999999998</v>
       </c>
       <c r="B45" s="21" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C45" s="21" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D45" s="23">
         <v>20</v>
@@ -3187,32 +3538,40 @@
         <v>0</v>
       </c>
       <c r="K45" s="23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L45" s="23">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M45" s="23">
         <v>5</v>
       </c>
-      <c r="N45" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="O45" s="24"/>
-      <c r="P45" s="52" t="str">
-        <f t="shared" ref="P45:P48" si="3">IF(O45=N45,"PASS","FAIL")</f>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="46" spans="1:17" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="N45" s="23">
+        <v>5</v>
+      </c>
+      <c r="O45" s="18">
+        <v>0</v>
+      </c>
+      <c r="P45" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q45" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="R45" s="52" t="str">
+        <f t="shared" ref="R45:R48" si="3">IF(Q45=P45,"PASS","FAIL")</f>
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A46" s="14">
         <v>2.4</v>
       </c>
       <c r="B46" s="16" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C46" s="16" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D46" s="18">
         <v>20</v>
@@ -3236,24 +3595,32 @@
         <v>0</v>
       </c>
       <c r="K46" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L46" s="18">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M46" s="18">
         <v>5</v>
       </c>
-      <c r="N46" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="O46" s="12"/>
-      <c r="P46" s="38" t="str">
+      <c r="N46" s="18">
+        <v>5</v>
+      </c>
+      <c r="O46" s="18">
+        <v>0</v>
+      </c>
+      <c r="P46" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q46" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="R46" s="38" t="str">
         <f t="shared" si="3"/>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="47" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="19"/>
       <c r="B47" s="21"/>
       <c r="C47" s="21"/>
@@ -3279,32 +3646,40 @@
         <v>0</v>
       </c>
       <c r="K47" s="23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L47" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M47" s="23">
         <v>0</v>
       </c>
-      <c r="N47" s="45" t="s">
-        <v>58</v>
-      </c>
-      <c r="O47" s="24"/>
-      <c r="P47" s="54" t="str">
+      <c r="N47" s="23">
+        <v>0</v>
+      </c>
+      <c r="O47" s="18">
+        <v>0</v>
+      </c>
+      <c r="P47" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q47" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="R47" s="54" t="str">
         <f t="shared" si="3"/>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="48" spans="1:17" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A48" s="14">
         <v>2.5</v>
       </c>
       <c r="B48" s="16" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C48" s="16" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D48" s="26">
         <v>20</v>
@@ -3328,67 +3703,75 @@
         <v>0</v>
       </c>
       <c r="K48" s="26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L48" s="26">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M48" s="26">
         <v>5</v>
       </c>
-      <c r="N48" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="O48" s="27"/>
-      <c r="P48" s="38" t="str">
+      <c r="N48" s="26">
+        <v>5</v>
+      </c>
+      <c r="O48" s="18">
+        <v>0</v>
+      </c>
+      <c r="P48" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q48" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="R48" s="38" t="str">
         <f t="shared" si="3"/>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.35">
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A53" s="68" t="s">
-        <v>1</v>
-      </c>
-      <c r="B53" s="70" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A53" s="67" t="s">
+        <v>1</v>
+      </c>
+      <c r="B53" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="C53" s="72" t="s">
+      <c r="C53" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="D53" s="74" t="s">
+      <c r="D53" s="75" t="s">
         <v>4</v>
       </c>
-      <c r="E53" s="75"/>
-      <c r="F53" s="75"/>
-      <c r="G53" s="75"/>
-      <c r="H53" s="75"/>
-      <c r="I53" s="75"/>
-      <c r="J53" s="75"/>
-      <c r="K53" s="75"/>
-      <c r="L53" s="75"/>
-      <c r="M53" s="76"/>
-      <c r="N53" s="64" t="s">
-        <v>5</v>
-      </c>
-      <c r="O53" s="64" t="s">
+      <c r="E53" s="76"/>
+      <c r="F53" s="76"/>
+      <c r="G53" s="76"/>
+      <c r="H53" s="76"/>
+      <c r="I53" s="76"/>
+      <c r="J53" s="76"/>
+      <c r="K53" s="76"/>
+      <c r="L53" s="76"/>
+      <c r="M53" s="77"/>
+      <c r="N53" s="73" t="s">
+        <v>5</v>
+      </c>
+      <c r="O53" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="P53" s="66" t="s">
+      <c r="P53" s="65" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A54" s="69"/>
-      <c r="B54" s="71"/>
-      <c r="C54" s="73"/>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A54" s="68"/>
+      <c r="B54" s="70"/>
+      <c r="C54" s="72"/>
       <c r="D54" s="4" t="s">
         <v>8</v>
       </c>
@@ -3419,19 +3802,19 @@
       <c r="M54" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="N54" s="65"/>
-      <c r="O54" s="65"/>
-      <c r="P54" s="67"/>
-    </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="N54" s="74"/>
+      <c r="O54" s="74"/>
+      <c r="P54" s="66"/>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" s="14">
         <v>3.1</v>
       </c>
       <c r="B55" s="16" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="D55" s="17">
         <v>20</v>
@@ -3464,7 +3847,7 @@
         <v>5</v>
       </c>
       <c r="N55" s="12" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="O55" s="11"/>
       <c r="P55" s="13" t="str">
@@ -3472,7 +3855,7 @@
         <v>FAIL</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" s="56"/>
       <c r="B56" s="16"/>
       <c r="C56" s="16"/>
@@ -3495,16 +3878,16 @@
         <v>15</v>
       </c>
       <c r="J56" s="55" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="K56" s="55" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="L56" s="55" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="M56" s="55" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="N56" s="41"/>
       <c r="O56" s="41"/>
@@ -3513,7 +3896,7 @@
         <v>PASS</v>
       </c>
     </row>
-    <row r="57" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="60"/>
       <c r="B57" s="21"/>
       <c r="C57" s="21"/>
@@ -3534,7 +3917,7 @@
         <v>PASS</v>
       </c>
     </row>
-    <row r="58" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A58" s="57"/>
       <c r="B58" s="58"/>
       <c r="C58" s="59"/>
@@ -3545,16 +3928,16 @@
         <v>9</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="G58" s="5" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="I58" s="5" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="J58" s="26"/>
       <c r="K58" s="26"/>
@@ -3567,13 +3950,13 @@
         <v>PASS</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" s="14">
         <v>3.2</v>
       </c>
       <c r="B59" s="50"/>
       <c r="C59" s="16" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="D59" s="18">
         <v>99</v>
@@ -3582,31 +3965,33 @@
         <v>99</v>
       </c>
       <c r="F59" s="55" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G59" s="55" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="H59" s="55" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="I59" s="55" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="J59" s="18"/>
       <c r="K59" s="18"/>
       <c r="L59" s="18"/>
       <c r="M59" s="18"/>
-      <c r="N59" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="O59" s="12"/>
+      <c r="N59" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="O59" s="12" t="s">
+        <v>85</v>
+      </c>
       <c r="P59" s="13" t="str">
         <f t="shared" si="4"/>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.35">
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="2"/>
       <c r="C60" s="3"/>
@@ -3617,16 +4002,16 @@
         <v>100</v>
       </c>
       <c r="F60" s="55" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G60" s="55" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="H60" s="55" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="I60" s="55" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="J60" s="18"/>
       <c r="K60" s="18"/>
@@ -3639,19 +4024,19 @@
         <v>PASS</v>
       </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A65" s="68" t="s">
-        <v>1</v>
-      </c>
-      <c r="B65" s="70" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A65" s="67" t="s">
+        <v>1</v>
+      </c>
+      <c r="B65" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="C65" s="72" t="s">
+      <c r="C65" s="71" t="s">
         <v>3</v>
       </c>
       <c r="D65" s="62" t="s">
@@ -3668,20 +4053,20 @@
       <c r="M65" s="62"/>
       <c r="N65" s="62"/>
       <c r="O65" s="62"/>
-      <c r="P65" s="64" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q65" s="64" t="s">
+      <c r="P65" s="73" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q65" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="R65" s="66" t="s">
+      <c r="R65" s="65" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A66" s="69"/>
-      <c r="B66" s="71"/>
-      <c r="C66" s="73"/>
+    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A66" s="68"/>
+      <c r="B66" s="70"/>
+      <c r="C66" s="72"/>
       <c r="D66" s="4" t="s">
         <v>8</v>
       </c>
@@ -3701,7 +4086,7 @@
         <v>13</v>
       </c>
       <c r="J66" s="5" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="K66" s="5" t="s">
         <v>14</v>
@@ -3716,21 +4101,21 @@
         <v>17</v>
       </c>
       <c r="O66" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="P66" s="65"/>
-      <c r="Q66" s="65"/>
-      <c r="R66" s="67"/>
-    </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.35">
+        <v>67</v>
+      </c>
+      <c r="P66" s="74"/>
+      <c r="Q66" s="74"/>
+      <c r="R66" s="66"/>
+    </row>
+    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A67" s="14">
         <v>4.0999999999999996</v>
       </c>
       <c r="B67" s="16" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="D67" s="17">
         <v>20</v>
@@ -3769,15 +4154,17 @@
         <v>0</v>
       </c>
       <c r="P67" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q67" s="11"/>
+        <v>87</v>
+      </c>
+      <c r="Q67" s="12" t="s">
+        <v>87</v>
+      </c>
       <c r="R67" s="13" t="str">
         <f>IF(P67=Q67,"PASS","FAIL")</f>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.35">
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A68" s="14"/>
       <c r="B68" s="16"/>
       <c r="C68" s="63"/>
@@ -3818,15 +4205,17 @@
         <v>0</v>
       </c>
       <c r="P68" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q68" s="11"/>
+        <v>88</v>
+      </c>
+      <c r="Q68" s="12" t="s">
+        <v>88</v>
+      </c>
       <c r="R68" s="13" t="str">
         <f t="shared" ref="R68:R76" si="5">IF(P68=Q68,"PASS","FAIL")</f>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.35">
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A69" s="14"/>
       <c r="B69" s="16"/>
       <c r="C69" s="63"/>
@@ -3867,15 +4256,17 @@
         <v>-1</v>
       </c>
       <c r="P69" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q69" s="11"/>
+        <v>88</v>
+      </c>
+      <c r="Q69" s="12" t="s">
+        <v>88</v>
+      </c>
       <c r="R69" s="13" t="str">
         <f t="shared" si="5"/>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.35">
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A70" s="14"/>
       <c r="B70" s="16"/>
       <c r="C70" s="63"/>
@@ -3916,15 +4307,17 @@
         <v>-1</v>
       </c>
       <c r="P70" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q70" s="11"/>
+        <v>88</v>
+      </c>
+      <c r="Q70" s="12" t="s">
+        <v>88</v>
+      </c>
       <c r="R70" s="13" t="str">
         <f t="shared" si="5"/>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.35">
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A71" s="14"/>
       <c r="B71" s="16"/>
       <c r="C71" s="63"/>
@@ -3965,15 +4358,17 @@
         <v>0</v>
       </c>
       <c r="P71" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q71" s="11"/>
+        <v>87</v>
+      </c>
+      <c r="Q71" s="12" t="s">
+        <v>87</v>
+      </c>
       <c r="R71" s="13" t="str">
         <f t="shared" si="5"/>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.35">
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A72" s="14"/>
       <c r="B72" s="16"/>
       <c r="C72" s="63"/>
@@ -4014,15 +4409,17 @@
         <v>999</v>
       </c>
       <c r="P72" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q72" s="11"/>
+        <v>87</v>
+      </c>
+      <c r="Q72" s="12" t="s">
+        <v>87</v>
+      </c>
       <c r="R72" s="13" t="str">
         <f t="shared" si="5"/>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.35">
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A73" s="14"/>
       <c r="B73" s="16"/>
       <c r="C73" s="63"/>
@@ -4063,15 +4460,17 @@
         <v>999</v>
       </c>
       <c r="P73" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q73" s="11"/>
+        <v>87</v>
+      </c>
+      <c r="Q73" s="12" t="s">
+        <v>87</v>
+      </c>
       <c r="R73" s="13" t="str">
         <f t="shared" si="5"/>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.35">
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A74" s="14"/>
       <c r="B74" s="16"/>
       <c r="C74" s="63"/>
@@ -4112,15 +4511,17 @@
         <v>999</v>
       </c>
       <c r="P74" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q74" s="11"/>
+        <v>88</v>
+      </c>
+      <c r="Q74" s="12" t="s">
+        <v>88</v>
+      </c>
       <c r="R74" s="13" t="str">
         <f t="shared" si="5"/>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.35">
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A75" s="14"/>
       <c r="B75" s="16"/>
       <c r="C75" s="63"/>
@@ -4161,15 +4562,17 @@
         <v>1000</v>
       </c>
       <c r="P75" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q75" s="12"/>
+        <v>88</v>
+      </c>
+      <c r="Q75" s="12" t="s">
+        <v>88</v>
+      </c>
       <c r="R75" s="13" t="str">
         <f t="shared" si="5"/>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.35">
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A76" s="14"/>
       <c r="B76" s="16"/>
       <c r="C76" s="63"/>
@@ -4210,32 +4613,126 @@
         <v>1000</v>
       </c>
       <c r="P76" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q76" s="12"/>
+        <v>88</v>
+      </c>
+      <c r="Q76" s="12" t="s">
+        <v>88</v>
+      </c>
       <c r="R76" s="13" t="str">
         <f t="shared" si="5"/>
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A77" s="14"/>
+      <c r="B77" s="16"/>
+      <c r="C77" s="63"/>
+      <c r="D77" s="17">
+        <v>20</v>
+      </c>
+      <c r="E77" s="18">
+        <v>20</v>
+      </c>
+      <c r="F77" s="18">
+        <v>0</v>
+      </c>
+      <c r="G77" s="18">
+        <v>0</v>
+      </c>
+      <c r="H77" s="18">
+        <v>10</v>
+      </c>
+      <c r="I77" s="18">
+        <v>15</v>
+      </c>
+      <c r="J77" s="18">
+        <v>0.1</v>
+      </c>
+      <c r="K77" s="18">
+        <v>0</v>
+      </c>
+      <c r="L77" s="18">
+        <v>1</v>
+      </c>
+      <c r="M77" s="18">
+        <v>5</v>
+      </c>
+      <c r="N77" s="18">
+        <v>5</v>
+      </c>
+      <c r="O77" s="18">
+        <v>0</v>
+      </c>
+      <c r="P77" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q77" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="R77" s="13" t="str">
+        <f t="shared" ref="R77" si="6">IF(P77=Q77,"PASS","FAIL")</f>
         <v>FAIL</v>
       </c>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="P77" s="38"/>
+    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A78" s="14"/>
+      <c r="B78" s="16"/>
+      <c r="C78" s="63"/>
+      <c r="D78" s="17">
+        <v>20</v>
+      </c>
+      <c r="E78" s="18">
+        <v>20</v>
+      </c>
+      <c r="F78" s="18">
+        <v>0</v>
+      </c>
+      <c r="G78" s="18">
+        <v>0</v>
+      </c>
+      <c r="H78" s="18">
+        <v>10</v>
+      </c>
+      <c r="I78" s="18">
+        <v>15</v>
+      </c>
+      <c r="J78" s="18">
+        <v>0</v>
+      </c>
+      <c r="K78" s="18">
+        <v>0</v>
+      </c>
+      <c r="L78" s="18">
+        <v>1</v>
+      </c>
+      <c r="M78" s="18">
+        <v>5</v>
+      </c>
+      <c r="N78" s="18">
+        <v>5</v>
+      </c>
+      <c r="O78" s="18">
+        <v>0.1</v>
+      </c>
+      <c r="P78" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q78" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="R78" s="13" t="str">
+        <f t="shared" ref="R78" si="7">IF(P78=Q78,"PASS","FAIL")</f>
+        <v>FAIL</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="N37:N38"/>
-    <mergeCell ref="O37:O38"/>
-    <mergeCell ref="P37:P38"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:M3"/>
-    <mergeCell ref="N3:N4"/>
-    <mergeCell ref="O3:O4"/>
+    <mergeCell ref="Q65:Q66"/>
+    <mergeCell ref="R65:R66"/>
+    <mergeCell ref="P65:P66"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="B65:B66"/>
+    <mergeCell ref="C65:C66"/>
     <mergeCell ref="N53:N54"/>
     <mergeCell ref="O53:O54"/>
     <mergeCell ref="P53:P54"/>
@@ -4243,35 +4740,42 @@
     <mergeCell ref="A53:A54"/>
     <mergeCell ref="B53:B54"/>
     <mergeCell ref="C53:C54"/>
-    <mergeCell ref="Q65:Q66"/>
-    <mergeCell ref="R65:R66"/>
-    <mergeCell ref="P65:P66"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="B65:B66"/>
-    <mergeCell ref="C65:C66"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="P37:P38"/>
+    <mergeCell ref="Q37:Q38"/>
+    <mergeCell ref="R37:R38"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="Q3:Q4"/>
+    <mergeCell ref="D3:O3"/>
   </mergeCells>
-  <conditionalFormatting sqref="P5:P33 P42 P45:P48">
+  <conditionalFormatting sqref="R5:R33 R42 R45:R48">
     <cfRule type="cellIs" dxfId="9" priority="43" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="8" priority="44" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",P5)))</formula>
+      <formula>NOT(ISERROR(SEARCH("PASS",R5)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P39:P41">
+  <conditionalFormatting sqref="R39:R41">
     <cfRule type="cellIs" dxfId="7" priority="31" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="6" priority="32" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",P39)))</formula>
+      <formula>NOT(ISERROR(SEARCH("PASS",R39)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P43:P44">
+  <conditionalFormatting sqref="R43:R44">
     <cfRule type="cellIs" dxfId="5" priority="29" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="4" priority="30" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",P43)))</formula>
+      <formula>NOT(ISERROR(SEARCH("PASS",R43)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P55:P60">
@@ -4282,7 +4786,7 @@
       <formula>NOT(ISERROR(SEARCH("PASS",P55)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R67:R76">
+  <conditionalFormatting sqref="R67:R78">
     <cfRule type="cellIs" dxfId="1" priority="21" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>

</xml_diff>